<commit_message>
Added box and whisker diagrams
</commit_message>
<xml_diff>
--- a/Dissertation_main/Dissertation_main/sheet_test_data_averages.xlsx
+++ b/Dissertation_main/Dissertation_main/sheet_test_data_averages.xlsx
@@ -909,11 +909,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T721"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:T121"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="22" max="22" width="24.25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5302,7 +5306,7 @@
         <v>19973</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:N127" si="8">AVERAGE(F67,F187,F307,F427,F547,F667)</f>
+        <f t="shared" ref="N67:N121" si="8">AVERAGE(F67,F187,F307,F427,F547,F667)</f>
         <v>2.5164</v>
       </c>
       <c r="O67">

</xml_diff>